<commit_message>
Updated code for ESSAVAILAIABLITYREQUEST TC
</commit_message>
<xml_diff>
--- a/Data/ESS Availability Pattern Requests and Manager Approval_CZ_REG.xlsx
+++ b/Data/ESS Availability Pattern Requests and Manager Approval_CZ_REG.xlsx
@@ -3,14 +3,27 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4EC6464-17C7-41FD-9244-72DCB525A190}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D672CC1-BF73-4BC1-A809-A070E46C82BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -472,7 +485,7 @@
   <dimension ref="A1:N10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>

</xml_diff>